<commit_message>
Add extra fields to fill + auto incrementing id.
</commit_message>
<xml_diff>
--- a/TechClub/Documents/applicants.xlsx
+++ b/TechClub/Documents/applicants.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="FirstRound" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Fname</t>
   </si>
@@ -57,51 +57,17 @@
     <t>WhatDoYouThinkOfThisForm</t>
   </si>
   <si>
-    <t>Abdelrahman</t>
-  </si>
-  <si>
-    <t>El Kinani</t>
-  </si>
-  <si>
-    <t>kinani95@outlook.com</t>
-  </si>
-  <si>
-    <t>Four</t>
-  </si>
-  <si>
-    <t>Computer_Science</t>
-  </si>
-  <si>
-    <t>Developers</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>awesome</t>
-  </si>
-  <si>
-    <t>Mostapha</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>mostapha@ahmed.alaa</t>
-  </si>
-  <si>
-    <t>WOW</t>
+    <t>AvailableOnDayX</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
@@ -462,127 +428,60 @@
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="26.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="38.7109375" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" customWidth="1"/>
+    <col min="14" max="14" width="36.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="N1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="0">
-        <v>20132052</v>
-      </c>
-      <c r="D2" s="0">
-        <v>1110780886</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="0">
-        <v>20132055</v>
-      </c>
-      <c r="D3" s="0">
-        <v>1110780886</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add thank you message after submit
</commit_message>
<xml_diff>
--- a/TechClub/Documents/applicants.xlsx
+++ b/TechClub/Documents/applicants.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="FirstRound" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>Id</t>
+  </si>
   <si>
     <t>Fname</t>
   </si>
@@ -51,23 +54,54 @@
     <t>BasicCoding</t>
   </si>
   <si>
+    <t>AvailableOnDayX</t>
+  </si>
+  <si>
     <t>GotSomethingElseToSay</t>
   </si>
   <si>
     <t>WhatDoYouThinkOfThisForm</t>
   </si>
   <si>
-    <t>AvailableOnDayX</t>
-  </si>
-  <si>
-    <t>Id</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>kinani95@outlook.com</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Computer_Science</t>
+  </si>
+  <si>
+    <t>Developers</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,7 +131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -437,51 +471,184 @@
     <col min="16" max="16" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
+      <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0">
+        <v>20302052</v>
+      </c>
+      <c r="E2" s="0">
+        <v>1110780886</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="0">
+        <v>20302052</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1110780886</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0">
+        <v>20302052</v>
+      </c>
+      <c r="E4" s="0">
+        <v>1110780886</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>